<commit_message>
HDS2-21 #time 15m ViewHelper und Test für "Maßstab" fetiggestellt (SingleRecordCartographicMathematicalData). Alle Tests erfolgreich. + neue Testtabelle
</commit_message>
<xml_diff>
--- a/tests/unit-tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/unit-tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -140,6 +140,56 @@
 </comments>
 </file>
 
+<file path=xl/comments14.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Erscheint das bei jedem Record?
+	-Sebastian Böttger</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments15.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Ist das ein "Entweder-Oder" oder ein "Wenn 502 $a nicht existiert, dann zeige 502 $b, $c, $d"-Oder?
+	-Sebastian Böttger</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
@@ -2568,238 +2618,27 @@
     <t xml:space="preserve">Geistiger Schöpfer / Konferenz</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">773 ist wiederholbar
+    <t xml:space="preserve">773 ist wiederholbar
 Die neuen Subfelder nach RDA sind bisher noch nicht in der Schnittstelle umgesetzt aber in Planung, 09.09.2016/nz
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="11"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">
 Suchlink generieren:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Wenn $w mit (DE-603) vorhanden
+Wenn $w mit (DE-603) vorhanden
 -&gt; Solr-Abfrage nach folgendem Schema:
-.....http://solr.hebis.de/verbund/select?wt=xml&amp;indent=true&amp;echoParams=none&amp;fq=</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">institution:ILN</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&amp;q=</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">id:HEB+PPN
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.....z.B. für die UB FFM: https://solr.hebis.de/verbund/select?wt=xml&amp;indent=true&amp;echoParams=none&amp;fq=</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">institution:3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&amp;q=</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">id:HEB046828966
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">-&gt; wenn Treffer &gt;0, dann Suchlink für die id-/PPN-Suche nach dem verknüpften Datensatz generieren: 
+.....http://solr.hebis.de/verbund/select?wt=xml&amp;indent=true&amp;echoParams=none&amp;fq=institution:ILN&amp;q=id:HEB+PPN
+.....z.B. für die UB FFM: https://solr.hebis.de/verbund/select?wt=xml&amp;indent=true&amp;echoParams=none&amp;fq=institution:3&amp;q=id:HEB046828966
+-&gt; wenn Treffer &gt;0, dann Suchlink für die id-/PPN-Suche nach dem verknüpften Datensatz generieren: 
 -&gt; PPN aus $w auslesen und "(DE-603)" durch "HEB" ersetzen
 -&gt; Suchlink daraus generieren nach folgendem Schema:
-.....https://fantasio.rz.uni-frankfurt.de/ubffm/Record/</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">HEB+PPN
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.....Beispiel PPN 246164956: https://fantasio.rz.uni-frankfurt.de/ubffm/Record/</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">HEB047408766
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">-&gt; diesen Link auf den Textstring aus $a und $t legen
+.....https://fantasio.rz.uni-frankfurt.de/ubffm/Record/HEB+PPN
+.....Beispiel PPN 246164956: https://fantasio.rz.uni-frankfurt.de/ubffm/Record/HEB047408766
+-&gt; diesen Link auf den Textstring aus $a und $t legen
 -&gt; Achtung: Wenn keine $w vorhanden ist bzw. bei 0 Treffern, nur Text anzeigen
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="11"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">
 Link/Button "alle Artikel anzeigen":
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">-&gt; PPN aus $w auslesen und "(DE-603)" entfernen
+-&gt; PPN aus $w auslesen und "(DE-603)" entfernen
 -&gt; Suchlink daraus generieren (Indexfeld "part of") nach folgendem Schema:
-     https://fantasio.rz.uni-frankfurt.de/ubffm/Search/Results?lookfor=</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">PPN</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&amp;type=part_of&amp;sort=pub_date_max+desc
-     Beispiel PPN 246164956: https://fantasio.rz.uni-frankfurt.de/ubffm/Search/Results?lookfor=</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">047408766</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&amp;type=part_of&amp;sort=pub_date_max+desc
+     https://fantasio.rz.uni-frankfurt.de/ubffm/Search/Results?lookfor=PPN&amp;type=part_of&amp;sort=pub_date_max+desc
+     Beispiel PPN 246164956: https://fantasio.rz.uni-frankfurt.de/ubffm/Search/Results?lookfor=047408766&amp;type=part_of&amp;sort=pub_date_max+desc
 -&gt; diesen Link auf den Textstring/Button "alle Artikel anzeigen" legen
 </t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">773 $t</t>
@@ -3134,7 +2973,7 @@
     <t xml:space="preserve">105439231</t>
   </si>
   <si>
-    <t xml:space="preserve">ISBN 3828812627 (Sekundärausgabe)</t>
+    <t xml:space="preserve">3828812627 (Sekundärausgabe)</t>
   </si>
   <si>
     <t xml:space="preserve">776 $z mit Indikator 1 = 1</t>
@@ -3229,7 +3068,7 @@
     <t xml:space="preserve">344651460</t>
   </si>
   <si>
-    <t xml:space="preserve">9790004341247 ; 9790004341254 ; 9790004341261 ; 9790004341278 ; 9790004341285</t>
+    <t xml:space="preserve">9790004341254 ; 9790004341261 ; 9790004341278 ; 9790004341285 ; 9790004341247</t>
   </si>
   <si>
     <t xml:space="preserve">024 $a mit Indikator 1 = 3</t>
@@ -3318,7 +3157,7 @@
     <t xml:space="preserve">371396379</t>
   </si>
   <si>
-    <t xml:space="preserve">0047-7238</t>
+    <t xml:space="preserve">0047-7238 ; 2397-7310</t>
   </si>
   <si>
     <t xml:space="preserve">Körperschaft</t>
@@ -7455,7 +7294,7 @@
   </sheetPr>
   <dimension ref="A1:Z28"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -9670,8 +9509,8 @@
   </sheetPr>
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10094,7 +9933,7 @@
       <c r="E35" s="33"/>
       <c r="F35" s="33"/>
     </row>
-    <row r="36" customFormat="false" ht="38.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="34" t="s">
         <v>333</v>
       </c>
@@ -10630,13 +10469,14 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="FFFF0000"/>
+    <tabColor rgb="FF00B050"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Z20"/>
@@ -10947,6 +10787,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -12435,8 +12276,8 @@
   </sheetPr>
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12622,7 +12463,7 @@
       <c r="E15" s="23"/>
       <c r="F15" s="24"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="19" t="s">
         <v>474</v>
       </c>
@@ -13261,7 +13102,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13461,7 +13302,7 @@
       <c r="E16" s="23"/>
       <c r="F16" s="24"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="19" t="s">
         <v>490</v>
       </c>

</xml_diff>

<commit_message>
HDS2-21 #time 40m ViewHelper und Test für "Schlagworte" fetiggestellt (SingleRecordSubjectAccessFieldsGeneralInformation). Alle Tests erfolgreich. + aktualisierte Tabelle
</commit_message>
<xml_diff>
--- a/tests/unit-tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/unit-tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="18"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -4754,7 +4754,8 @@
     <t xml:space="preserve">212739271</t>
   </si>
   <si>
-    <t xml:space="preserve">Vereinte Nationen / Charter of the United Nations
+    <t xml:space="preserve">Japan / Verfassung
+Vereinte Nationen / Charter of the United Nations
 Begriff
 Armee
 Kollektive Sicherheit
@@ -12276,7 +12277,7 @@
   </sheetPr>
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -14890,8 +14891,8 @@
   </sheetPr>
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D57" activeCellId="0" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15578,7 +15579,7 @@
       <c r="E57" s="23"/>
       <c r="F57" s="24"/>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="75.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="19" t="s">
         <v>626</v>
       </c>

</xml_diff>

<commit_message>
cleanup / unit tests
</commit_message>
<xml_diff>
--- a/tests/unit-tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/unit-tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="13"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -796,7 +796,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2026" uniqueCount="1147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2026" uniqueCount="1148">
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
@@ -1432,7 +1432,7 @@
     <t xml:space="preserve">047322551</t>
   </si>
   <si>
-    <t xml:space="preserve">Mikrofiche-Ausg.:: München : Bayerische Staatsbibliothek, 1997. 260 Mikrofiches : 24x. - Mikrofilm-Ausg.: München : Bayerische Staatsbibliothek, 1997. Preservation und Printing Master. Je 13 Rollfilme. - Mikrofilm-Ausg.: Berlin : Staatsbibliothek zu Berlin</t>
+    <t xml:space="preserve">Mikrofiche-Ausg.: München : Bayerische Staatsbibliothek, 1997. 260 Mikrofiches : 24x. - Mikrofilm-Ausg.: München : Bayerische Staatsbibliothek, 1997. Preservation und Printing Master. Je 13 Rollfilme. - Mikrofilm-Ausg.: Berlin : Staatsbibliothek zu Berlin</t>
   </si>
   <si>
     <t xml:space="preserve">Ausgabe</t>
@@ -6642,6 +6642,9 @@
   </si>
   <si>
     <t xml:space="preserve">Riga, 1904</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Riga : Stahl</t>
   </si>
   <si>
     <t xml:space="preserve">2x $a</t>
@@ -10473,7 +10476,7 @@
   </sheetPr>
   <dimension ref="A1:Z28"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -19246,8 +19249,8 @@
   </sheetPr>
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19407,7 +19410,7 @@
       <c r="E13" s="36"/>
       <c r="F13" s="36"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="49.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="37" t="s">
         <v>108</v>
       </c>
@@ -20445,8 +20448,8 @@
   </sheetPr>
   <dimension ref="A1:Z24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20675,7 +20678,7 @@
       </c>
       <c r="F18" s="24"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="19" t="s">
         <v>188</v>
       </c>
@@ -20687,7 +20690,7 @@
         <v>954</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="F19" s="24"/>
     </row>
@@ -20705,39 +20708,39 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="19" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="B21" s="38" t="s">
         <v>194</v>
       </c>
       <c r="C21" s="21"/>
       <c r="D21" s="22" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="F21" s="24"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="19" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="B22" s="38" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="22" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="F22" s="24"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="19" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B23" s="38" t="s">
         <v>127</v>
@@ -20745,7 +20748,7 @@
       <c r="C23" s="21"/>
       <c r="D23" s="22"/>
       <c r="E23" s="23" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="F23" s="24"/>
       <c r="G23" s="62"/>
@@ -20771,7 +20774,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="37" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="B24" s="38" t="s">
         <v>545</v>
@@ -20781,7 +20784,7 @@
         <v>550</v>
       </c>
       <c r="E24" s="41" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="F24" s="42"/>
     </row>
@@ -20825,7 +20828,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="C1" s="26"/>
       <c r="D1" s="26"/>
@@ -20837,7 +20840,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
@@ -20913,7 +20916,7 @@
         <v>166</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>327</v>
@@ -20927,7 +20930,7 @@
         <v>169</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="3"/>
@@ -20939,7 +20942,7 @@
         <v>171</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="3"/>
@@ -20994,42 +20997,42 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="37" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="B16" s="38" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="C16" s="39"/>
       <c r="D16" s="40" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="E16" s="41"/>
       <c r="F16" s="42"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="37" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="C17" s="39"/>
       <c r="D17" s="40" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="E17" s="41"/>
       <c r="F17" s="42"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="37" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="B18" s="38" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="C18" s="39"/>
       <c r="D18" s="40" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="E18" s="41"/>
       <c r="F18" s="42"/>
@@ -21073,7 +21076,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="C1" s="26"/>
       <c r="D1" s="26"/>
@@ -21085,7 +21088,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
@@ -21097,7 +21100,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="C3" s="26"/>
       <c r="D3" s="26"/>
@@ -21161,10 +21164,10 @@
         <v>105</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -21172,10 +21175,10 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="31" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="3"/>
@@ -21184,10 +21187,10 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="31" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="3"/>
@@ -21208,7 +21211,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="31" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="B13" s="34" t="s">
         <v>49</v>
@@ -21220,7 +21223,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="31" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="B14" s="34" t="s">
         <v>738</v>
@@ -21232,10 +21235,10 @@
     </row>
     <row r="15" customFormat="false" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="31" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="3"/>
@@ -21290,14 +21293,14 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="43" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="B20" s="44" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="C20" s="45"/>
       <c r="D20" s="46" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E20" s="47"/>
       <c r="F20" s="48"/>
@@ -21324,56 +21327,56 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="37" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B21" s="38" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C21" s="39"/>
       <c r="D21" s="40" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E21" s="41"/>
       <c r="F21" s="42"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="37" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="B22" s="38" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="C22" s="39"/>
       <c r="D22" s="40" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="E22" s="41"/>
       <c r="F22" s="42"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="37" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="C23" s="39"/>
       <c r="D23" s="40" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="E23" s="41"/>
       <c r="F23" s="42"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="37" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="B24" s="38" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="C24" s="39"/>
       <c r="D24" s="40" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="E24" s="41"/>
       <c r="F24" s="42"/>
@@ -21419,7 +21422,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C1" s="26"/>
       <c r="D1" s="26"/>
@@ -21431,7 +21434,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
@@ -21443,7 +21446,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="C3" s="26"/>
       <c r="D3" s="26"/>
@@ -21510,7 +21513,7 @@
         <v>307</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -21518,10 +21521,10 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="31" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="3"/>
@@ -21530,10 +21533,10 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="31" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="3"/>
@@ -21542,7 +21545,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="31" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="B12" s="32" t="s">
         <v>710</v>
@@ -21554,10 +21557,10 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="31" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="3"/>
@@ -21566,10 +21569,10 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="31" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="3"/>
@@ -21578,10 +21581,10 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="31" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="3"/>
@@ -21590,10 +21593,10 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="31" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="3"/>
@@ -21602,10 +21605,10 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="31" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="3"/>
@@ -21614,10 +21617,10 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="31" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="3"/>
@@ -21626,7 +21629,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="31" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="B19" s="34" t="s">
         <v>622</v>
@@ -21638,10 +21641,10 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="31" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="3"/>
@@ -21650,10 +21653,10 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="31" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="3"/>
@@ -21662,7 +21665,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="31" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="B22" s="32" t="s">
         <v>710</v>
@@ -21674,10 +21677,10 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="31" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="3"/>
@@ -21686,10 +21689,10 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="31" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="B24" s="34" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="3"/>
@@ -21698,10 +21701,10 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="31" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="3"/>
@@ -21710,10 +21713,10 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="31" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="3"/>
@@ -21722,10 +21725,10 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="31" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="B27" s="34" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="3"/>
@@ -21734,10 +21737,10 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="31" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="B28" s="34" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="3"/>
@@ -21746,7 +21749,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="31" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="B29" s="34" t="s">
         <v>622</v>
@@ -21758,10 +21761,10 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="31" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -21769,7 +21772,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="31" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="B31" s="32" t="s">
         <v>710</v>
@@ -21780,10 +21783,10 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="31" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
@@ -21791,10 +21794,10 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="31" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="B33" s="32" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
@@ -21802,7 +21805,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="31" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="B34" s="32" t="s">
         <v>710</v>
@@ -21813,10 +21816,10 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="31" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="B35" s="32" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
@@ -21824,10 +21827,10 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="31" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="B36" s="32" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
@@ -21835,10 +21838,10 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="31" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="B37" s="32" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
@@ -21846,10 +21849,10 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="31" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="B38" s="32" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
@@ -21857,10 +21860,10 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="31" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="B39" s="32" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
@@ -21868,10 +21871,10 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="31" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="B40" s="32" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
@@ -21879,7 +21882,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="31" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="B41" s="32" t="s">
         <v>622</v>
@@ -21890,10 +21893,10 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="31" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="B42" s="32" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
@@ -21901,10 +21904,10 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="31" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="B43" s="32" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
@@ -21912,7 +21915,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="31" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="B44" s="32" t="s">
         <v>710</v>
@@ -21923,10 +21926,10 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="31" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="B45" s="32" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
@@ -21934,10 +21937,10 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="31" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="B46" s="32" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
@@ -21945,10 +21948,10 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="31" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="B47" s="32" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
@@ -21956,10 +21959,10 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="31" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="B48" s="32" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
@@ -21967,10 +21970,10 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="31" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="B49" s="32" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
@@ -21978,10 +21981,10 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="31" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="B50" s="32" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
@@ -21989,7 +21992,7 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="31" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="B51" s="32" t="s">
         <v>622</v>
@@ -22000,10 +22003,10 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="31" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="B52" s="32" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
@@ -22011,10 +22014,10 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="31" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="B53" s="32" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
@@ -22033,10 +22036,10 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="31" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="B55" s="32" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
@@ -22044,10 +22047,10 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="31" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="B56" s="32" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
@@ -22058,7 +22061,7 @@
         <v>479</v>
       </c>
       <c r="B57" s="32" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
@@ -22066,10 +22069,10 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="31" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="B58" s="32" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
@@ -22077,10 +22080,10 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="31" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="B59" s="32" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
@@ -22088,10 +22091,10 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="31" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="B60" s="32" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
@@ -22099,7 +22102,7 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="31" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="B61" s="32" t="s">
         <v>622</v>
@@ -22110,10 +22113,10 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="31" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="B62" s="32" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
@@ -22121,10 +22124,10 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="31" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="B63" s="32" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
@@ -22143,10 +22146,10 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="31" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="B65" s="32" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
@@ -22154,10 +22157,10 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="31" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="B66" s="32" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
@@ -22168,7 +22171,7 @@
         <v>484</v>
       </c>
       <c r="B67" s="32" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
@@ -22176,10 +22179,10 @@
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="31" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="B68" s="32" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
@@ -22187,10 +22190,10 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="31" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="B69" s="32" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
@@ -22198,10 +22201,10 @@
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="31" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="B70" s="32" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
@@ -22209,7 +22212,7 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="31" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="B71" s="32" t="s">
         <v>622</v>
@@ -22266,70 +22269,70 @@
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="37" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="B76" s="38" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="C76" s="39"/>
       <c r="D76" s="40" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="E76" s="41"/>
       <c r="F76" s="42"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="37" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="B77" s="38" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="C77" s="39"/>
       <c r="D77" s="40" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="E77" s="41"/>
       <c r="F77" s="42"/>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="37" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="B78" s="38" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="C78" s="39"/>
       <c r="D78" s="40" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="E78" s="41"/>
       <c r="F78" s="42"/>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="37" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="B79" s="38" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="C79" s="39"/>
       <c r="D79" s="40" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="E79" s="41"/>
       <c r="F79" s="42"/>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="37" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="B80" s="38" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="C80" s="39"/>
       <c r="D80" s="40" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="E80" s="41"/>
       <c r="F80" s="42"/>
@@ -22339,109 +22342,109 @@
         <v>934</v>
       </c>
       <c r="B81" s="38" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="C81" s="39"/>
       <c r="D81" s="40" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="E81" s="41"/>
       <c r="F81" s="42"/>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="37" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="B82" s="38" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="C82" s="39"/>
       <c r="D82" s="40" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="E82" s="41"/>
       <c r="F82" s="42"/>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="37" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="B83" s="38" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="C83" s="39"/>
       <c r="D83" s="40" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="E83" s="41"/>
       <c r="F83" s="42"/>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="37" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="B84" s="38" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C84" s="39"/>
       <c r="D84" s="40" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="E84" s="41"/>
       <c r="F84" s="42"/>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="37" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="B85" s="38" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="C85" s="39"/>
       <c r="D85" s="40" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="E85" s="41"/>
       <c r="F85" s="42"/>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="37" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B86" s="38" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="C86" s="39"/>
       <c r="D86" s="40" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="E86" s="41"/>
       <c r="F86" s="42"/>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="37" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="B87" s="38" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="C87" s="39"/>
       <c r="D87" s="40" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="E87" s="41"/>
       <c r="F87" s="42"/>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="37" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="B88" s="38" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="C88" s="39"/>
       <c r="D88" s="40" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="E88" s="41"/>
       <c r="F88" s="42"/>
@@ -22451,95 +22454,95 @@
         <v>934</v>
       </c>
       <c r="B89" s="38" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="C89" s="39"/>
       <c r="D89" s="40" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="E89" s="41"/>
       <c r="F89" s="42"/>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="37" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="B90" s="38" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="C90" s="39"/>
       <c r="D90" s="40" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="E90" s="41"/>
       <c r="F90" s="42"/>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="37" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="B91" s="38" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="C91" s="39"/>
       <c r="D91" s="40" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="E91" s="41"/>
       <c r="F91" s="42"/>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="37" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="B92" s="38" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="C92" s="39"/>
       <c r="D92" s="40" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="E92" s="41"/>
       <c r="F92" s="42"/>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="37" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="B93" s="38" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="C93" s="39"/>
       <c r="D93" s="40" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="E93" s="41"/>
       <c r="F93" s="42"/>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="37" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="B94" s="38" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="C94" s="39"/>
       <c r="D94" s="40" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="E94" s="41"/>
       <c r="F94" s="42"/>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="37" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="B95" s="38" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="C95" s="39"/>
       <c r="D95" s="40" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="E95" s="41"/>
       <c r="F95" s="42"/>
@@ -22583,7 +22586,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="C1" s="53"/>
       <c r="D1" s="53"/>
@@ -22595,7 +22598,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="C2" s="53"/>
       <c r="D2" s="53"/>
@@ -22607,7 +22610,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="C3" s="26"/>
       <c r="D3" s="26"/>
@@ -22668,13 +22671,13 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="3"/>
@@ -22682,10 +22685,10 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -22740,42 +22743,42 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="19" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="B15" s="38" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="C15" s="21"/>
       <c r="D15" s="22" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="E15" s="23"/>
       <c r="F15" s="24"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="19" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="B16" s="38" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C16" s="21"/>
       <c r="D16" s="22" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="E16" s="23"/>
       <c r="F16" s="24"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="19" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="C17" s="21"/>
       <c r="D17" s="22" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="E17" s="23"/>
       <c r="F17" s="24"/>
@@ -22819,7 +22822,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="C1" s="26"/>
       <c r="D1" s="26"/>
@@ -22829,7 +22832,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>

</xml_diff>

<commit_message>
HDS2-88 Einzeltrefferanzeige: diverse Anzeigefehler
</commit_message>
<xml_diff>
--- a/tests/unit-tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/unit-tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="17"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -750,7 +750,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2022" uniqueCount="1098">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2024" uniqueCount="1096">
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
@@ -1750,13 +1750,13 @@
     <t xml:space="preserve">383651484</t>
   </si>
   <si>
-    <t xml:space="preserve">[Entstehungsort nicht ermittelbar], 18.07.1620, 18.07.1620</t>
+    <t xml:space="preserve">[Entstehungsort nicht ermittelbar], 18.07.1620</t>
   </si>
   <si>
     <t xml:space="preserve">383650747</t>
   </si>
   <si>
-    <t xml:space="preserve">[Entstehungsort nicht ermittelbar], 20.06.1620, 20.06.1620</t>
+    <t xml:space="preserve">[Entstehungsort nicht ermittelbar], 20.06.1620</t>
   </si>
   <si>
     <t xml:space="preserve">Erscheingunsjahr</t>
@@ -2352,8 +2352,8 @@
     <t xml:space="preserve">2x 780</t>
   </si>
   <si>
-    <t xml:space="preserve">Vorg.: Büchereidienst
-Darin aufgeg.: Deutscher Büchereiverband: Kurzinformationen</t>
+    <t xml:space="preserve">Darin aufgeg.: Deutscher Büchereiverband: Kurzinformationen
+Vorg.: Büchereidienst</t>
   </si>
   <si>
     <t xml:space="preserve">046829962</t>
@@ -2387,7 +2387,7 @@
     <t xml:space="preserve">381476669</t>
   </si>
   <si>
-    <t xml:space="preserve">Vorausgabe: Rettungsdienst heute. - ISBN 9783437461934</t>
+    <t xml:space="preserve">Vorausgegangen ist: Rettungsdienst heute. - ISBN 9783437461934</t>
   </si>
   <si>
     <t xml:space="preserve">780 mit $t $d + 040 $e = rda, ohne $a</t>
@@ -2917,7 +2917,7 @@
     <t xml:space="preserve">2x 020 $a</t>
   </si>
   <si>
-    <t xml:space="preserve">9782070451609 ; 2070451607</t>
+    <t xml:space="preserve">2070451607 ; 9782070451609</t>
   </si>
   <si>
     <t xml:space="preserve">2x 020 $a + 1x 020 $z</t>
@@ -2926,7 +2926,7 @@
     <t xml:space="preserve">312333870</t>
   </si>
   <si>
-    <t xml:space="preserve">9783861432036 ; 9783861432039 ; 386143203X</t>
+    <t xml:space="preserve">386143203X ; 9783861432036 ; 9783861432039</t>
   </si>
   <si>
     <t xml:space="preserve">020 $a mit Sekundärausgabe</t>
@@ -3030,7 +3030,7 @@
     <t xml:space="preserve">344651460</t>
   </si>
   <si>
-    <t xml:space="preserve">9790004341254 ; 9790004341261 ; 9790004341278 ; 9790004341285 ; 9790004341247</t>
+    <t xml:space="preserve">9790004341247 ; 9790004341254 ; 9790004341261 ; 9790004341278 ; 9790004341285</t>
   </si>
   <si>
     <t xml:space="preserve">024 $a mit Indikator 1 = 3</t>
@@ -3884,6 +3884,7 @@
         <color rgb="FF000000"/>
         <rFont val="SimSun"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">于阳 </t>
     </r>
@@ -3931,6 +3932,7 @@
         <color rgb="FF000000"/>
         <rFont val="SimSun"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">郭道晖 </t>
     </r>
@@ -3950,6 +3952,7 @@
         <color rgb="FF000000"/>
         <rFont val="SimSun"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">刘永艳 </t>
     </r>
@@ -3994,6 +3997,7 @@
         <color rgb="FF000000"/>
         <rFont val="SimSun"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">北京 </t>
     </r>
@@ -4013,6 +4017,7 @@
         <color rgb="FF000000"/>
         <rFont val="SimSun"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">当代中国出版社</t>
     </r>
@@ -4060,6 +4065,7 @@
         <color rgb="FF000000"/>
         <rFont val="SimSun"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">江湖中国 </t>
     </r>
@@ -4079,6 +4085,7 @@
         <color rgb="FF000000"/>
         <rFont val="SimSun"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">一个非正式制度在中国的起因 </t>
     </r>
@@ -4098,6 +4105,7 @@
         <color rgb="FF000000"/>
         <rFont val="SimSun"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">于阳著</t>
     </r>
@@ -4823,11 +4831,11 @@
     <t xml:space="preserve">104075848</t>
   </si>
   <si>
-    <t xml:space="preserve">Spinoza, Benedictus _x0098_de
-Geschichte Anfänge -1800
+    <t xml:space="preserve">Spinoza, Benedictus de
 Rezeption
 Deutschland
-Aufsatzsammlung</t>
+Aufsatzsammlung
+Geschichte Anfänge -1800</t>
   </si>
   <si>
     <t xml:space="preserve">610 $a $b $g $b $b</t>
@@ -4837,10 +4845,9 @@
   </si>
   <si>
     <t xml:space="preserve">Universitätsbibliothek Heidelberg / Salem &lt;Bodenseekreis&gt; / Kloster / Bibliothek
-Geschichte 1500-1900
 Handschrift
 Katalog
-</t>
+Geschichte 1500-1900</t>
   </si>
   <si>
     <t xml:space="preserve">Kleist, Heinrich von
@@ -4869,14 +4876,31 @@
     <t xml:space="preserve">04567986X</t>
   </si>
   <si>
-    <t xml:space="preserve">Karl V. &lt;Heiliges Römisches Reich, Kaiser&gt;
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Karl V. &lt;Heiliges Römisches Reich, Kaiser&gt;
 Valdivia, Pedro de
-Geschichte 1500-1554
 Chile, Eroberung
 Chile
 Briefsammlung
 Quelle
 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Geschichte 1500-1554</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">650 mit @</t>
@@ -5735,14 +5759,14 @@
   </si>
   <si>
     <t xml:space="preserve">Flowering plants volumes
-Vol. 16. Fabaceae / ed. by O. A. Leistner ...
-Pt. 2 / ed. by J. H. Ross</t>
+Vol. 16. Fabaceae  / ed. by O. A. Leistner ...
+Pt. 2  / ed. by J. H. Ross</t>
   </si>
   <si>
     <t xml:space="preserve">Leader Pos. 19 = c mit 245</t>
   </si>
   <si>
-    <t xml:space="preserve">Reihe A. Die Porträtsammlung der Herzog-August-Bibliothek Wolfenbüttel / bearb. von Peter Mortzfeld
+    <t xml:space="preserve">Reihe A. Die Porträtsammlung der Herzog-August-Bibliothek Wolfenbüttel  / bearb. von Peter Mortzfeld
 Bd. 17. Abbildungen Nas - Pao</t>
   </si>
   <si>
@@ -5972,64 +5996,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Jiang hu Zhong guo : yi ge fei zheng shi zhi du zai Zhong guo de qi yin / Yu Yang zhu
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">江湖中国 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">一个非正式制度在中国的起因 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">/ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">于阳著</t>
-    </r>
+    <t xml:space="preserve">Jiang hu Zhong guo : yi ge fei zheng shi zhi du zai Zhong guo de qi yin / Yu Yang zhu</t>
   </si>
   <si>
     <t xml:space="preserve">Jiang hu Zhong guo : yi ge fei zheng shi zhi du zai Zhong guo de qi yin</t>
@@ -6490,6 +6457,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Yu, Yang (Verfasser)</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -6498,41 +6468,6 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Yu, Yang (Verfasser)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">于阳 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(Verfasser)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Yu, Yang (Verfasser)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
       <t xml:space="preserve">100 und 700 mit Originalschrift in 880
 </t>
     </r>
@@ -6548,55 +6483,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Guo, Daohui (Verfasser); Liu, Yongyan (Verfasser)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">郭道晖 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(Verfasser); </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">刘永艳 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(Verfasser)</t>
-    </r>
+    <t xml:space="preserve">Guo, Daohui (Verfasser); Liu, Yongyan (Verfasser)</t>
   </si>
   <si>
     <t xml:space="preserve">Guo, Daohui (Verfasser)</t>
@@ -6708,57 +6595,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Bei jing : Dang dai zhong guo chu ban she, 2016
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">北京 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">当代中国出版社</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">, 2016</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Bei jing : Dang dai zhong guo chu ban she, 2016</t>
   </si>
   <si>
@@ -6983,7 +6819,7 @@
     <t xml:space="preserve">120323435</t>
   </si>
   <si>
-    <t xml:space="preserve">Stuttgart : Belser, [19]89. - 6 Mikrofiches. - (Edition Corvey : Deutschsprachige Belletristik)</t>
+    <t xml:space="preserve">Stuttgart : Belser, 1989, [19]89. - 6 Mikrofiches. - (Edition Corvey : Deutschsprachige Belletristik)</t>
   </si>
   <si>
     <t xml:space="preserve">530 $a + 533 $b - $e</t>
@@ -7493,7 +7329,7 @@
     <t xml:space="preserve">381940063</t>
   </si>
   <si>
-    <t xml:space="preserve">Ab 10 Jahren</t>
+    <t xml:space="preserve">Kind, 10-12 Jahre</t>
   </si>
   <si>
     <t xml:space="preserve">RecordFinder</t>
@@ -7541,7 +7377,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -7659,6 +7495,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="SimSun"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -8273,15 +8116,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.0279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.5720930232558"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.7209302325581"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.7860465116279"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.4558139534884"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.893023255814"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.2046511627907"/>
-    <col collapsed="false" hidden="false" max="26" min="8" style="0" width="9.45116279069767"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.1813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.1162790697674"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="56.8372093023256"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.2"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.4744186046512"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.2232558139535"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.6976744186047"/>
+    <col collapsed="false" hidden="false" max="26" min="8" style="0" width="10.3720930232558"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9158,18 +9001,18 @@
   </sheetPr>
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2046511627907"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.9488372093023"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.2418604651163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="52.6372093023256"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.5906976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.6976744186047"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="59.3302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.3627906976744"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.7581395348837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.2976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9582,7 +9425,7 @@
       <c r="E35" s="36"/>
       <c r="F35" s="36"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="25.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="44" t="s">
         <v>307</v>
       </c>
@@ -9624,7 +9467,7 @@
       <c r="E38" s="48"/>
       <c r="F38" s="49"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="44" t="s">
         <v>314</v>
       </c>
@@ -9638,7 +9481,7 @@
       <c r="E39" s="48"/>
       <c r="F39" s="49"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="44" t="s">
         <v>317</v>
       </c>
@@ -9693,11 +9536,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.1720930232558"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.0186046511628"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.4046511627907"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.8790697674419"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.7953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.5627906976744"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.293023255814"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.7395348837209"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9942,11 +9785,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.1209302325581"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.7348837209302"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.5860465116279"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.0697674418605"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.6139534883721"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.0186046511628"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.6046511627907"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10134,12 +9977,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.5953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.6046511627907"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.5395348837209"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.5395348837209"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.2093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.8837209302326"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1162790697674"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="55.3953488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.493023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10451,12 +10294,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.7302325581395"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.4046511627907"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.5395348837209"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.6046511627907"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.8651162790698"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.2232558139535"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.2651162790698"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1162790697674"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.8837209302326"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.1488372093023"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10860,18 +10703,18 @@
   </sheetPr>
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.8093023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.5395348837209"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="52.1116279069767"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.6046511627907"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.1720930232558"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.2790697674419"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1162790697674"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.2325581395349"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.8837209302326"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11046,7 +10889,7 @@
       <c r="E15" s="36"/>
       <c r="F15" s="14"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="19" t="s">
         <v>407</v>
       </c>
@@ -11060,7 +10903,7 @@
       <c r="E16" s="23"/>
       <c r="F16" s="24"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="19" t="s">
         <v>409</v>
       </c>
@@ -11156,17 +10999,17 @@
   </sheetPr>
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.8604651162791"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.5953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.5395348837209"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.9255813953488"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.353488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1162790697674"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1255813953488"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11343,7 +11186,7 @@
       <c r="E15" s="23"/>
       <c r="F15" s="24"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="19" t="s">
         <v>429</v>
       </c>
@@ -11418,11 +11261,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.7302325581395"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.4651162790698"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.5395348837209"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.1813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.2232558139535"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.9581395348837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1162790697674"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.5906976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11681,18 +11524,18 @@
   </sheetPr>
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D46" activeCellId="0" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8883720930233"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="76.2651162790698"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.5395348837209"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.5906976744186"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.8651162790698"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.1209302325581"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="83.7488372093023"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1162790697674"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.4"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.1488372093023"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12283,17 +12126,17 @@
   </sheetPr>
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.8093023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.7348837209302"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.4837209302326"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.1720930232558"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.0186046511628"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.2790697674419"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.2418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12444,8 +12287,10 @@
       <c r="E13" s="36"/>
       <c r="F13" s="36"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="44"/>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="44" t="s">
+        <v>519</v>
+      </c>
       <c r="B14" s="45" t="s">
         <v>521</v>
       </c>
@@ -12456,8 +12301,10 @@
       <c r="E14" s="48"/>
       <c r="F14" s="49"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="44"/>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="44" t="s">
+        <v>519</v>
+      </c>
       <c r="B15" s="45" t="s">
         <v>523</v>
       </c>
@@ -12494,11 +12341,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.9906976744186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.0139534883721"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.1209302325581"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.4046511627907"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.4837209302326"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.8697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.6139534883721"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="55.2651162790698"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13112,11 +12959,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.0697674418605"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.7348837209302"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.5302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.1441860465116"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.5674418604651"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.0186046511628"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.6"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="55"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13341,11 +13188,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.5395348837209"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="59.7255813953488"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.5395348837209"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.3627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1162790697674"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.6325581395349"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1162790697674"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.906976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13556,9 +13403,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.5395348837209"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.4"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1162790697674"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.4697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13760,18 +13607,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2046511627907"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.0325581395349"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.7348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.6976744186047"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.8697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.0186046511628"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13938,19 +13785,20 @@
       <c r="E14" s="48"/>
       <c r="F14" s="49"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="78" t="s">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="37.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="78" t="s">
         <v>551</v>
       </c>
-      <c r="B15" s="79" t="s">
+      <c r="B17" s="79" t="s">
         <v>552</v>
       </c>
-      <c r="C15" s="80"/>
-      <c r="D15" s="81" t="s">
+      <c r="C17" s="80"/>
+      <c r="D17" s="81" t="s">
         <v>553</v>
       </c>
-      <c r="E15" s="48"/>
-      <c r="F15" s="82"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="82"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -13976,11 +13824,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2046511627907"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.9674418604651"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.9255813953488"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.846511627907"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.6976744186047"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.5116279069767"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.1255813953488"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.8651162790698"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14179,18 +14027,18 @@
   </sheetPr>
   <dimension ref="A1:Z69"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D58" activeCellId="0" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.7302325581395"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.153488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.5395348837209"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.4558139534884"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.7348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.2232558139535"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.4883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1162790697674"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.5767441860465"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.0186046511628"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14827,7 +14675,7 @@
       <c r="E53" s="36"/>
       <c r="F53" s="14"/>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="61.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="58" t="s">
         <v>637</v>
       </c>
@@ -14861,7 +14709,7 @@
       <c r="Y54" s="43"/>
       <c r="Z54" s="43"/>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="61.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="58" t="s">
         <v>640</v>
       </c>
@@ -14963,7 +14811,7 @@
       <c r="Y57" s="43"/>
       <c r="Z57" s="43"/>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="85.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="58" t="s">
         <v>619</v>
       </c>
@@ -15169,13 +15017,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.0697674418605"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.1069767441861"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.353488372093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="63.9255813953488"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.4651162790698"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.7302325581395"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.5674418604651"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.4372093023256"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.1116279069767"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="70.2279069767442"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.9581395348837"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.2232558139535"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16210,11 +16058,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.4651162790698"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.7348837209302"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.2046511627907"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.5953488372093"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.9581395348837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.0186046511628"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.6976744186047"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16412,20 +16260,20 @@
   </sheetPr>
   <dimension ref="A1:Z16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.4139534883721"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.153488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.4046511627907"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.5813953488372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.6790697674419"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.0744186046512"/>
-    <col collapsed="false" hidden="false" max="26" min="7" style="0" width="9.45116279069767"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.7767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.4883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.2651162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.9116279069767"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.0418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.2558139534884"/>
+    <col collapsed="false" hidden="false" max="26" min="7" style="0" width="10.3720930232558"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16938,18 +16786,18 @@
   </sheetPr>
   <dimension ref="A1:Z28"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E35" activeCellId="0" sqref="E35"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.5953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.7348837209302"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.2604651162791"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.8558139534884"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="49.7488372093023"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.0186046511628"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.5441860465116"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.6604651162791"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="54.6046511627907"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17836,7 +17684,7 @@
       <c r="Y27" s="89"/>
       <c r="Z27" s="89"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="26.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="44" t="s">
         <v>835</v>
       </c>
@@ -17881,11 +17729,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2046511627907"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.7348837209302"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.2186046511628"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.0604651162791"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.6976744186047"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.0186046511628"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.2883720930233"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.0511627906977"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18074,14 +17922,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.5488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.4139534883721"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.1906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.6976744186047"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.4139534883721"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.8093023255814"/>
-    <col collapsed="false" hidden="false" max="26" min="7" style="0" width="9.45116279069767"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.9116279069767"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.7767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.2093023255814"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.4558139534884"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.7767441860465"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.1720930232558"/>
+    <col collapsed="false" hidden="false" max="26" min="7" style="0" width="10.3720930232558"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19536,10 +19384,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="25.0697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.5953488372093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.7348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="27.5674418604651"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.093023255814"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.0186046511628"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19809,14 +19657,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.153488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.5720930232558"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.9953488372093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.9302325581395"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.5488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.2837209302326"/>
-    <col collapsed="false" hidden="false" max="26" min="7" style="0" width="9.45116279069767"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.5162790697674"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.1162790697674"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.5860465116279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.8186046511628"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.9116279069767"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.646511627907"/>
+    <col collapsed="false" hidden="false" max="26" min="7" style="0" width="10.3720930232558"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -20321,18 +20169,18 @@
   </sheetPr>
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.3348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.9255813953488"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.4744186046512"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.8790697674419"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.6046511627907"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.8279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.1255813953488"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.753488372093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.7395348837209"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.8837209302326"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20723,7 +20571,7 @@
       </c>
       <c r="F30" s="49"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="26.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="44" t="s">
         <v>922</v>
       </c>
@@ -20735,23 +20583,23 @@
         <v>923</v>
       </c>
       <c r="E31" s="48" t="s">
+        <v>923</v>
+      </c>
+      <c r="F31" s="49"/>
+    </row>
+    <row r="32" customFormat="false" ht="38.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="44" t="s">
         <v>924</v>
-      </c>
-      <c r="F31" s="49"/>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="44" t="s">
-        <v>925</v>
       </c>
       <c r="B32" s="45" t="s">
         <v>536</v>
       </c>
       <c r="C32" s="46"/>
       <c r="D32" s="47" t="s">
+        <v>925</v>
+      </c>
+      <c r="E32" s="48" t="s">
         <v>926</v>
-      </c>
-      <c r="E32" s="48" t="s">
-        <v>927</v>
       </c>
       <c r="F32" s="49"/>
     </row>
@@ -20777,18 +20625,18 @@
   </sheetPr>
   <dimension ref="A1:Z24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.5953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.6139534883721"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.5395348837209"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.7348837209302"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.8651162790698"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="68.7813953488372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1162790697674"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.0186046511628"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.1488372093023"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20796,7 +20644,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="C1" s="53"/>
       <c r="D1" s="53"/>
@@ -20808,7 +20656,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="C2" s="53"/>
       <c r="D2" s="53"/>
@@ -20884,10 +20732,10 @@
         <v>165</v>
       </c>
       <c r="B9" s="12" t="s">
+        <v>929</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>930</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>931</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="3"/>
@@ -20898,7 +20746,7 @@
         <v>168</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -20919,10 +20767,10 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
+        <v>932</v>
+      </c>
+      <c r="B12" s="12" t="s">
         <v>933</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>934</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -20984,10 +20832,10 @@
       </c>
       <c r="C17" s="21"/>
       <c r="D17" s="22" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="F17" s="24"/>
     </row>
@@ -21000,10 +20848,10 @@
       </c>
       <c r="C18" s="21"/>
       <c r="D18" s="22" t="s">
+        <v>935</v>
+      </c>
+      <c r="E18" s="23" t="s">
         <v>936</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>937</v>
       </c>
       <c r="F18" s="24"/>
     </row>
@@ -21016,10 +20864,10 @@
       </c>
       <c r="C19" s="21"/>
       <c r="D19" s="22" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="F19" s="24"/>
     </row>
@@ -21037,39 +20885,39 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="19" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="B21" s="45" t="s">
         <v>193</v>
       </c>
       <c r="C21" s="21"/>
       <c r="D21" s="22" t="s">
+        <v>939</v>
+      </c>
+      <c r="E21" s="23" t="s">
         <v>940</v>
-      </c>
-      <c r="E21" s="23" t="s">
-        <v>941</v>
       </c>
       <c r="F21" s="24"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="19" t="s">
+        <v>941</v>
+      </c>
+      <c r="B22" s="45" t="s">
         <v>942</v>
-      </c>
-      <c r="B22" s="45" t="s">
-        <v>943</v>
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="22" t="s">
+        <v>943</v>
+      </c>
+      <c r="E22" s="23" t="s">
         <v>944</v>
-      </c>
-      <c r="E22" s="23" t="s">
-        <v>945</v>
       </c>
       <c r="F22" s="24"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="19" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B23" s="45" t="s">
         <v>128</v>
@@ -21077,7 +20925,7 @@
       <c r="C23" s="21"/>
       <c r="D23" s="22"/>
       <c r="E23" s="23" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="F23" s="24"/>
       <c r="G23" s="63"/>
@@ -21101,19 +20949,19 @@
       <c r="Y23" s="63"/>
       <c r="Z23" s="63"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="26.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="44" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="B24" s="45" t="s">
         <v>533</v>
       </c>
       <c r="C24" s="46"/>
       <c r="D24" s="47" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="E24" s="48" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="F24" s="49"/>
     </row>
@@ -21145,11 +20993,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.5953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.6232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.2046511627907"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.6046511627907"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.1674418604651"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.6976744186047"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.8837209302326"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21157,7 +21005,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="C1" s="26"/>
       <c r="D1" s="26"/>
@@ -21169,7 +21017,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
@@ -21245,7 +21093,7 @@
         <v>165</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>326</v>
@@ -21259,7 +21107,7 @@
         <v>168</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="3"/>
@@ -21271,7 +21119,7 @@
         <v>170</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="3"/>
@@ -21326,42 +21174,42 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="44" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="B16" s="45" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="C16" s="46"/>
       <c r="D16" s="47" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="E16" s="48"/>
       <c r="F16" s="49"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="44" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="B17" s="45" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="C17" s="46"/>
       <c r="D17" s="47" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="E17" s="48"/>
       <c r="F17" s="49"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="44" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="B18" s="45" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="C18" s="46"/>
       <c r="D18" s="47" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="E18" s="48"/>
       <c r="F18" s="49"/>
@@ -21388,16 +21236,16 @@
   </sheetPr>
   <dimension ref="A1:Z27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.5953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.4558139534884"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="50.6697674418605"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.5767441860465"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="55.6558139534884"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21405,7 +21253,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="C1" s="26"/>
       <c r="D1" s="26"/>
@@ -21417,7 +21265,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
@@ -21429,7 +21277,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="C3" s="26"/>
       <c r="D3" s="26"/>
@@ -21493,10 +21341,10 @@
         <v>106</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -21504,10 +21352,10 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="31" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="3"/>
@@ -21516,10 +21364,10 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="31" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="3"/>
@@ -21528,7 +21376,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="31" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="B12" s="32" t="s">
         <v>593</v>
@@ -21540,7 +21388,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="31" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="B13" s="34" t="s">
         <v>49</v>
@@ -21552,7 +21400,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="31" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="B14" s="34" t="s">
         <v>729</v>
@@ -21564,10 +21412,10 @@
     </row>
     <row r="15" customFormat="false" ht="86.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="31" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="3"/>
@@ -21620,16 +21468,16 @@
       <c r="E19" s="36"/>
       <c r="F19" s="36"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="37" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="B20" s="38" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="C20" s="39"/>
       <c r="D20" s="40" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="E20" s="41"/>
       <c r="F20" s="42"/>
@@ -21666,56 +21514,56 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="44" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="B24" s="45" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="C24" s="46"/>
       <c r="D24" s="47" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="E24" s="48"/>
       <c r="F24" s="49"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="44" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="B25" s="45" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="C25" s="46"/>
       <c r="D25" s="47" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="E25" s="48"/>
       <c r="F25" s="49"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="44" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="B26" s="45" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="C26" s="46"/>
       <c r="D26" s="47" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="E26" s="48"/>
       <c r="F26" s="49"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="44" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="B27" s="45" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="C27" s="46"/>
       <c r="D27" s="47" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="E27" s="48"/>
       <c r="F27" s="49"/>
@@ -21749,12 +21597,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2046511627907"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.1069767441861"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4279069767442"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="67.4697674418605"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.1953488372093"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.6976744186047"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.4372093023256"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.2651162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="74.1674418604651"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.9023255813954"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21762,7 +21610,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="C1" s="26"/>
       <c r="D1" s="26"/>
@@ -21774,7 +21622,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
@@ -21786,7 +21634,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="C3" s="26"/>
       <c r="D3" s="26"/>
@@ -21853,7 +21701,7 @@
         <v>306</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -21861,10 +21709,10 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="31" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="3"/>
@@ -21873,10 +21721,10 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="31" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="3"/>
@@ -21885,7 +21733,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="31" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="B12" s="32" t="s">
         <v>701</v>
@@ -21897,10 +21745,10 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="31" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="3"/>
@@ -21909,10 +21757,10 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="31" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="3"/>
@@ -21921,10 +21769,10 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="31" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="3"/>
@@ -21933,10 +21781,10 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="31" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="3"/>
@@ -21945,10 +21793,10 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="31" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="3"/>
@@ -21957,10 +21805,10 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="31" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="3"/>
@@ -21969,7 +21817,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="31" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="B19" s="34" t="s">
         <v>612</v>
@@ -21981,10 +21829,10 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="31" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="3"/>
@@ -21993,10 +21841,10 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="31" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="3"/>
@@ -22005,7 +21853,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="31" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="B22" s="32" t="s">
         <v>701</v>
@@ -22017,10 +21865,10 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="31" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="3"/>
@@ -22029,10 +21877,10 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="31" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="B24" s="34" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="3"/>
@@ -22041,10 +21889,10 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="31" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="3"/>
@@ -22053,10 +21901,10 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="31" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="3"/>
@@ -22065,10 +21913,10 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="31" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="B27" s="34" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="3"/>
@@ -22077,10 +21925,10 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="31" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="B28" s="34" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="3"/>
@@ -22089,7 +21937,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="31" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="B29" s="34" t="s">
         <v>612</v>
@@ -22101,10 +21949,10 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="31" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -22112,7 +21960,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="31" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="B31" s="32" t="s">
         <v>701</v>
@@ -22123,10 +21971,10 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="31" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
@@ -22134,10 +21982,10 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="31" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="B33" s="32" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
@@ -22145,7 +21993,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="31" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="B34" s="32" t="s">
         <v>701</v>
@@ -22156,10 +22004,10 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="31" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="B35" s="32" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
@@ -22167,10 +22015,10 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="31" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="B36" s="32" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
@@ -22178,10 +22026,10 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="31" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="B37" s="32" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
@@ -22189,10 +22037,10 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="31" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="B38" s="32" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
@@ -22200,10 +22048,10 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="31" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="B39" s="32" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
@@ -22211,10 +22059,10 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="31" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="B40" s="32" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
@@ -22222,7 +22070,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="31" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="B41" s="32" t="s">
         <v>612</v>
@@ -22233,10 +22081,10 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="31" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="B42" s="32" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
@@ -22244,10 +22092,10 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="31" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="B43" s="32" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
@@ -22255,7 +22103,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="31" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="B44" s="32" t="s">
         <v>701</v>
@@ -22266,10 +22114,10 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="31" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="B45" s="32" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
@@ -22277,10 +22125,10 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="31" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="B46" s="32" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
@@ -22288,10 +22136,10 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="31" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="B47" s="32" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
@@ -22299,10 +22147,10 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="31" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="B48" s="32" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
@@ -22310,10 +22158,10 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="31" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="B49" s="32" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
@@ -22321,10 +22169,10 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="31" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="B50" s="32" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
@@ -22332,7 +22180,7 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="31" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="B51" s="32" t="s">
         <v>612</v>
@@ -22343,10 +22191,10 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="31" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="B52" s="32" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
@@ -22354,10 +22202,10 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="31" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="B53" s="32" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
@@ -22376,10 +22224,10 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="31" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="B55" s="32" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
@@ -22387,10 +22235,10 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="31" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="B56" s="32" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
@@ -22401,7 +22249,7 @@
         <v>476</v>
       </c>
       <c r="B57" s="32" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
@@ -22409,10 +22257,10 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="31" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="B58" s="32" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
@@ -22420,10 +22268,10 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="31" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="B59" s="32" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
@@ -22431,10 +22279,10 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="31" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="B60" s="32" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
@@ -22442,7 +22290,7 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="31" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="B61" s="32" t="s">
         <v>612</v>
@@ -22453,10 +22301,10 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="31" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="B62" s="32" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
@@ -22464,10 +22312,10 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="31" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="B63" s="32" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
@@ -22486,10 +22334,10 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="31" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="B65" s="32" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
@@ -22497,10 +22345,10 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="31" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="B66" s="32" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
@@ -22511,7 +22359,7 @@
         <v>481</v>
       </c>
       <c r="B67" s="32" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
@@ -22519,10 +22367,10 @@
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="31" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="B68" s="32" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
@@ -22530,10 +22378,10 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="31" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="B69" s="32" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
@@ -22541,10 +22389,10 @@
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="31" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="B70" s="32" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
@@ -22552,7 +22400,7 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="31" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="B71" s="32" t="s">
         <v>612</v>
@@ -22609,112 +22457,112 @@
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="44" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="B76" s="45" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="C76" s="46"/>
       <c r="D76" s="47" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="E76" s="48"/>
       <c r="F76" s="49"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="44" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="B77" s="45" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="C77" s="46"/>
       <c r="D77" s="47" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="E77" s="48"/>
       <c r="F77" s="49"/>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="44" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="B78" s="45" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="C78" s="46"/>
       <c r="D78" s="47" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="E78" s="48"/>
       <c r="F78" s="49"/>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="44" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="B79" s="45" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="C79" s="46"/>
       <c r="D79" s="47" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="E79" s="48"/>
       <c r="F79" s="49"/>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="44" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="B80" s="45" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="C80" s="46"/>
       <c r="D80" s="47" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="E80" s="48"/>
       <c r="F80" s="49"/>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="44" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="B81" s="45" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="C81" s="46"/>
       <c r="D81" s="47" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="E81" s="48"/>
       <c r="F81" s="49"/>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="44" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="B82" s="45" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="C82" s="46"/>
       <c r="D82" s="47" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="E82" s="48"/>
       <c r="F82" s="49"/>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="44" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="B83" s="45" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="C83" s="46"/>
       <c r="D83" s="47" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="E83" s="48"/>
       <c r="F83" s="49"/>
@@ -22742,16 +22590,16 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.5953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.7302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.5395348837209"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.6046511627907"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.2232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1162790697674"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.8837209302326"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22759,7 +22607,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="C1" s="53"/>
       <c r="D1" s="53"/>
@@ -22771,7 +22619,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="C2" s="53"/>
       <c r="D2" s="53"/>
@@ -22783,7 +22631,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="C3" s="26"/>
       <c r="D3" s="26"/>
@@ -22844,13 +22692,13 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>1085</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>1086</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>1087</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="3"/>
@@ -22858,10 +22706,10 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -22916,42 +22764,42 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="19" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="B15" s="45" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="C15" s="21"/>
       <c r="D15" s="22" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="E15" s="23"/>
       <c r="F15" s="24"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="19" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="B16" s="45" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="C16" s="21"/>
       <c r="D16" s="22" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="E16" s="23"/>
       <c r="F16" s="24"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="19" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="B17" s="45" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="C17" s="21"/>
       <c r="D17" s="22" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="E17" s="23"/>
       <c r="F17" s="24"/>
@@ -22984,10 +22832,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.0697674418605"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.3395348837209"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.9488372093023"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.5674418604651"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="74.0325581395349"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.2279069767442"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22995,7 +22843,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="C1" s="26"/>
       <c r="D1" s="26"/>
@@ -23005,7 +22853,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
@@ -23067,9 +22915,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.5860465116279"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.5720930232558"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.6046511627907"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.1162790697674"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23308,14 +23156,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.2837209302326"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.5906976744186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.8651162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.5488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.6790697674419"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.5488372093023"/>
-    <col collapsed="false" hidden="false" max="26" min="7" style="0" width="9.45116279069767"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.646511627907"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.4"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.1488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.0139534883721"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.0418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.9116279069767"/>
+    <col collapsed="false" hidden="false" max="26" min="7" style="0" width="10.3720930232558"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -25125,16 +24973,16 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2046511627907"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.8651162790698"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.1767441860465"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.9255813953488"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.6976744186047"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.1488372093023"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.9023255813953"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1255813953488"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25309,7 +25157,7 @@
       <c r="E15" s="36"/>
       <c r="F15" s="36"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="44" t="s">
         <v>172</v>
       </c>
@@ -25323,7 +25171,7 @@
       <c r="E16" s="48"/>
       <c r="F16" s="49"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="44" t="s">
         <v>172</v>
       </c>
@@ -25364,9 +25212,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.5953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.9302325581395"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.9209302325581"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25613,11 +25461,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.6976744186047"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.3720930232558"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.3348837209302"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.2046511627907"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.4558139534884"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.3906976744186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.8279069767442"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.6976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25821,12 +25669,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.1720930232558"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.0186046511628"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.9813953488372"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.0697674418605"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.7581395348837"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="16.5395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.7953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.6651162790698"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.1023255813954"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5674418604651"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.9906976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="18.1162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>